<commit_message>
Update Unit assessment worksheet.xlsx
</commit_message>
<xml_diff>
--- a/Woodbadge-S7-427-17/!Ticket/Ticket3/Unit assessment worksheet.xlsx
+++ b/Woodbadge-S7-427-17/!Ticket/Ticket3/Unit assessment worksheet.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt.ballance\Documents\GitHub\Scouting\Woodbadge-S7-427-17\!Ticket\Ticket3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76FB4E2C-A2F3-4D38-A6D8-F176DDED8801}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97B70D9-CE50-4DB2-8552-CA07B6ACD6DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="24720" windowHeight="12210" activeTab="6" xr2:uid="{6B70A27B-6F48-42E2-ACBD-7E65943473BE}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7530" firstSheet="5" activeTab="11" xr2:uid="{6B70A27B-6F48-42E2-ACBD-7E65943473BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Committee" sheetId="1" r:id="rId1"/>
-    <sheet name="Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Training" sheetId="8" r:id="rId3"/>
-    <sheet name="Advancement" sheetId="3" r:id="rId4"/>
-    <sheet name="Finances" sheetId="4" r:id="rId5"/>
-    <sheet name="CO Relations" sheetId="5" r:id="rId6"/>
-    <sheet name="Recruitment&amp;Retention" sheetId="6" r:id="rId7"/>
-    <sheet name="Lists" sheetId="7" r:id="rId8"/>
+    <sheet name="Introduction" sheetId="12" r:id="rId1"/>
+    <sheet name="Unit Committee" sheetId="1" r:id="rId2"/>
+    <sheet name="Unit Training" sheetId="8" r:id="rId3"/>
+    <sheet name="Unit Finances" sheetId="4" r:id="rId4"/>
+    <sheet name="Unit-CO Relations" sheetId="5" r:id="rId5"/>
+    <sheet name="BSA Program" sheetId="2" r:id="rId6"/>
+    <sheet name="BSA Advancement" sheetId="3" r:id="rId7"/>
+    <sheet name="BSA Recruitment&amp;Retention" sheetId="6" r:id="rId8"/>
+    <sheet name="CS Program" sheetId="9" r:id="rId9"/>
+    <sheet name="CS Advancement" sheetId="10" r:id="rId10"/>
+    <sheet name="CS Recruitment&amp;Retention" sheetId="11" r:id="rId11"/>
+    <sheet name="Lists" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>This section is designed to ask questions about the unit committee and it's operations</t>
   </si>
@@ -120,30 +124,12 @@
     <t>This section asks questions about the program being delivered to the youth</t>
   </si>
   <si>
-    <t>How often does the unit meet?</t>
-  </si>
-  <si>
-    <t>How often does the unit have an outdoor experience</t>
-  </si>
-  <si>
-    <t>Does the unit follow the boy-led model?</t>
-  </si>
-  <si>
-    <t>Does the unit have an active PLC?</t>
-  </si>
-  <si>
-    <t>How far in advance does the unit plan meetings?</t>
-  </si>
-  <si>
     <t>Are meeting agendas provided to the scouts on a regular basis?</t>
   </si>
   <si>
     <t>How often are service projects scheduled?</t>
   </si>
   <si>
-    <t>Does the unit participate in the JTE program?</t>
-  </si>
-  <si>
     <t>B3</t>
   </si>
   <si>
@@ -195,9 +181,6 @@
     <t>No Planning</t>
   </si>
   <si>
-    <t>Does the unit have a plan for providing the program to differently-abled participants?</t>
-  </si>
-  <si>
     <t xml:space="preserve">This section focuses on the adult and youth training for leaders. </t>
   </si>
   <si>
@@ -232,6 +215,105 @@
   </si>
   <si>
     <t>This section focuses on the unit's recruitment and retention of new and existing members</t>
+  </si>
+  <si>
+    <t>How often does the troop meet?</t>
+  </si>
+  <si>
+    <t>How often does the troop have an outdoor experience</t>
+  </si>
+  <si>
+    <t>Does the troop follow the boy-led model?</t>
+  </si>
+  <si>
+    <t>Does the troop have an active PLC?</t>
+  </si>
+  <si>
+    <t>How far in advance does the troop plan meetings?</t>
+  </si>
+  <si>
+    <t>Does the troop participate in the JTE program?</t>
+  </si>
+  <si>
+    <t>Does the troop have a plan for providing the program to differently-abled participants?</t>
+  </si>
+  <si>
+    <t>How many of the youth members have advanced at least one rank in the year?</t>
+  </si>
+  <si>
+    <t>How many scouts attend summer camp?</t>
+  </si>
+  <si>
+    <t>How many scouts attend Merit Badge College?</t>
+  </si>
+  <si>
+    <t>Are scoutbook records being updated properly and synced?</t>
+  </si>
+  <si>
+    <t>Does the troop have a relationship with a cub scout pack?</t>
+  </si>
+  <si>
+    <t>Does the troop have a policy of contacting "missing" scouts to determine what is going on?</t>
+  </si>
+  <si>
+    <t>Does the troop actively promote their activites in the community?</t>
+  </si>
+  <si>
+    <t>This section focuses on the Cub Scout program, both at the Den and Pack level</t>
+  </si>
+  <si>
+    <t>Pack Program</t>
+  </si>
+  <si>
+    <t>How often does the pack hold a pack meeting?</t>
+  </si>
+  <si>
+    <t>How often are advancement and awards presented to the cubs?</t>
+  </si>
+  <si>
+    <t>Does the unit's chartered organization provide an account for the unit?</t>
+  </si>
+  <si>
+    <t>Does the unit have a dues assessment for the unit's use?</t>
+  </si>
+  <si>
+    <t>How often does the committee treasurer provide an financial update?</t>
+  </si>
+  <si>
+    <t>Does the Charter Partner provide any funding to the unit?</t>
+  </si>
+  <si>
+    <t>Does the unit offer camperships or hardship funding for youth in need?</t>
+  </si>
+  <si>
+    <t>Doe the COR attend unit committee meetings?</t>
+  </si>
+  <si>
+    <t>Does the Unit Leader and Committee Chair meet with the COR outside the scheduled committee meetings?</t>
+  </si>
+  <si>
+    <t>Does the Institution Head take an active role in the unit?</t>
+  </si>
+  <si>
+    <t>Does the unit prepare an annual budget?</t>
+  </si>
+  <si>
+    <t>How often does the unit track current spending/income to the budget?</t>
+  </si>
+  <si>
+    <t>Does the unit have a unit debit card?</t>
+  </si>
+  <si>
+    <t>Are there controls in place to require two signatures/approvals to withdraw funds?</t>
+  </si>
+  <si>
+    <t>How much can be withdrawn from a unit account without committee approval (petty cash)?</t>
+  </si>
+  <si>
+    <t>This workbook is designed to help you find areas of conern with the units you are responsible for. It doesn't cover all situations, and you should be verifying any recommendations that are made. Not all sections will apply to all units, and are color-coded to the program.</t>
+  </si>
+  <si>
+    <t>Yellow tabs are universal, Red tabs apply to ScoutsBSA, Blue tabs are for the Cub Scouting Program.</t>
   </si>
 </sst>
 </file>
@@ -267,9 +349,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,6 +668,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304E5C17-0B9C-429C-9399-47BBA4547843}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8426BB2F-7B2A-4C53-B4FC-992AB7FCCBBD}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22390BA2-A89F-4BD5-B80A-3681C02AFF77}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C910F9-75D5-4278-8052-70B386A9DB23}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5657E4D-497E-4BE6-B1D6-8C3F18100D78}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -590,7 +1055,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,12 +1151,332 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45EA4216-6536-4916-99CB-7E50A7CD262B}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E1A203B-3715-43E3-B6B6-7564D758487D}">
+          <x14:formula1>
+            <xm:f>Lists!$Q$2:$Q$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83061E64-52B2-43A3-9B3D-E5DD7D377B18}">
+          <x14:formula1>
+            <xm:f>Lists!$R$2:$R$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D1303A-8C86-47CC-AB36-4F4CE8E6918D}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3166B7-E7C6-46E3-8B6A-C45C04E6BA1E}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799E1DF0-34EF-4A6B-B5CC-FA7FF407445C}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,47 +1491,47 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -814,149 +1599,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45EA4216-6536-4916-99CB-7E50A7CD262B}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABE9E36-0B47-4379-8F26-AD7C935C1EF8}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E1A203B-3715-43E3-B6B6-7564D758487D}">
-          <x14:formula1>
-            <xm:f>Lists!$Q$2:$Q$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83061E64-52B2-43A3-9B3D-E5DD7D377B18}">
-          <x14:formula1>
-            <xm:f>Lists!$R$2:$R$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABE9E36-0B47-4379-8F26-AD7C935C1EF8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D1303A-8C86-47CC-AB36-4F4CE8E6918D}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3166B7-E7C6-46E3-8B6A-C45C04E6BA1E}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAF1BBE-FF00-4E64-B621-E6411C4DF1F3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -965,256 +1646,83 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C910F9-75D5-4278-8052-70B386A9DB23}">
-  <dimension ref="A1:R7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAF1BBE-FF00-4E64-B621-E6411C4DF1F3}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" t="s">
-        <v>46</v>
-      </c>
-      <c r="N6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFD67FD-832B-4E32-BF0A-0DBAD23508FA}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Ticket Package Updates
</commit_message>
<xml_diff>
--- a/Woodbadge-S7-427-17/!Ticket/Ticket3/Unit assessment worksheet.xlsx
+++ b/Woodbadge-S7-427-17/!Ticket/Ticket3/Unit assessment worksheet.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt.ballance\Documents\GitHub\Scouting\Woodbadge-S7-427-17\!Ticket\Ticket3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97B70D9-CE50-4DB2-8552-CA07B6ACD6DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADC9463-A479-4651-ADAC-A6E51A684368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7530" firstSheet="5" activeTab="11" xr2:uid="{6B70A27B-6F48-42E2-ACBD-7E65943473BE}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7530" activeTab="11" xr2:uid="{6B70A27B-6F48-42E2-ACBD-7E65943473BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="12" r:id="rId1"/>
     <sheet name="Unit Committee" sheetId="1" r:id="rId2"/>
     <sheet name="Unit Training" sheetId="8" r:id="rId3"/>
-    <sheet name="Unit Finances" sheetId="4" r:id="rId4"/>
-    <sheet name="Unit-CO Relations" sheetId="5" r:id="rId5"/>
+    <sheet name="Unit-CO Relations" sheetId="5" r:id="rId4"/>
+    <sheet name="Unit Finances" sheetId="4" r:id="rId5"/>
     <sheet name="BSA Program" sheetId="2" r:id="rId6"/>
     <sheet name="BSA Advancement" sheetId="3" r:id="rId7"/>
     <sheet name="BSA Recruitment&amp;Retention" sheetId="6" r:id="rId8"/>
     <sheet name="CS Program" sheetId="9" r:id="rId9"/>
     <sheet name="CS Advancement" sheetId="10" r:id="rId10"/>
     <sheet name="CS Recruitment&amp;Retention" sheetId="11" r:id="rId11"/>
-    <sheet name="Lists" sheetId="7" r:id="rId12"/>
+    <sheet name="Recommendations" sheetId="13" r:id="rId12"/>
+    <sheet name="Lists" sheetId="7" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="137">
   <si>
     <t>This section is designed to ask questions about the unit committee and it's operations</t>
   </si>
@@ -202,9 +203,6 @@
     <t>Does the unit have a representative attend Roundtable?</t>
   </si>
   <si>
-    <t xml:space="preserve">Are all direct-contact leaders trained for outdoor activities? (BALOO, IOLS, Etc.) </t>
-  </si>
-  <si>
     <t>This section focuses on the advancement of the youth members</t>
   </si>
   <si>
@@ -314,13 +312,157 @@
   </si>
   <si>
     <t>Yellow tabs are universal, Red tabs apply to ScoutsBSA, Blue tabs are for the Cub Scouting Program.</t>
+  </si>
+  <si>
+    <t>Does the pack participate in the Summer Outdoor Experience Program?</t>
+  </si>
+  <si>
+    <t>Does the pack attend council camping events?</t>
+  </si>
+  <si>
+    <t>Does the pack have functioning dens?</t>
+  </si>
+  <si>
+    <t>This section focuses on the Advancement of the youth in the pack</t>
+  </si>
+  <si>
+    <t>Den Program</t>
+  </si>
+  <si>
+    <t>Are dens structured in accordance with BSA Recommended practices?</t>
+  </si>
+  <si>
+    <t>Are the den leaders trained?</t>
+  </si>
+  <si>
+    <t>Do dens conduct regular meetings outside the pack meetings?</t>
+  </si>
+  <si>
+    <t>Are den meetings planned beforehand?</t>
+  </si>
+  <si>
+    <t>Do dens meet to complete adventures on a regular basis?</t>
+  </si>
+  <si>
+    <t>Do new members earn their bobcat award within the appropriate time period?</t>
+  </si>
+  <si>
+    <t>What percentage of the dens advance to the next rank on time?</t>
+  </si>
+  <si>
+    <t>Are advancement records updated and posted in ScoutBook?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are there leaders trained for outdoor activities? (BALOO, IOLS, Etc.) </t>
+  </si>
+  <si>
+    <t>Every Meeting</t>
+  </si>
+  <si>
+    <t>Type of unit</t>
+  </si>
+  <si>
+    <t>Unit Number</t>
+  </si>
+  <si>
+    <t>Registered Youth</t>
+  </si>
+  <si>
+    <t>Registered Adults</t>
+  </si>
+  <si>
+    <t>Troop</t>
+  </si>
+  <si>
+    <t>Registered Committee</t>
+  </si>
+  <si>
+    <t>Registered Direct Contact</t>
+  </si>
+  <si>
+    <t>Number of Patrols</t>
+  </si>
+  <si>
+    <t>75%-85%</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Is there a committee position focused on recruitement/retention?</t>
+  </si>
+  <si>
+    <t>You may want to make sure that members of the committee have an opportunity to cycle off more frequently to prevent burn-out.</t>
+  </si>
+  <si>
+    <t>Training is a critical part of delivering a quality program. Make sure these leaders complete their leader-specific training.</t>
+  </si>
+  <si>
+    <t>Depending on your situation, you may need to implement an assessment to fund your unit. Also, having a vested interest may help scouts stay more active.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depending on your situation, having a mechanism to assist scouts in need can increase participation levels. </t>
+  </si>
+  <si>
+    <t>Ideally, the committee would be reviewing the budget tracking each meeting.</t>
+  </si>
+  <si>
+    <t>The use of a "debit card" for petty cash allows for some flexibility, but appropriate controls must be in place. Discuss this item with your COR.</t>
+  </si>
+  <si>
+    <t>Depending on the size of your unit, you may need to allocate more funding for emergency purchases (advancement, registrations, etc..)</t>
+  </si>
+  <si>
+    <t>Planning farther in advance will allow you to have more consistent unit meetings. Consider an annual plan that is flexible enough to change as needed.</t>
+  </si>
+  <si>
+    <t>Giving scouts, and their parents/guardians, a "heads up" on what will be going on at the meetings can improve your participation and the preparedness of your scouts.</t>
+  </si>
+  <si>
+    <t>If you are able to make reasonable accomodations, having a plan for inclusion will increase your unit numbers, and allow you to reach more of the youth that need our program the most.</t>
+  </si>
+  <si>
+    <t>Ideally, we should see every scout advance at least one rank within the year. Monitor these numbers and make sure they aren't declining.</t>
+  </si>
+  <si>
+    <t>Summer camp is a perfect opportunity to allow scouts to bond, experiment with various interests, and build self-confidence. Look at why these numbers aren't 100% and look for opportunities to increase these numbers.</t>
+  </si>
+  <si>
+    <t>After conducting the assessment, the following areas are areas of concern. Red items are of the highest importance and should be resolved as soon as possible.</t>
+  </si>
+  <si>
+    <t>Meeting at least quarterly (monthly or bi-monthly would be better) will allow for the committee to identify issues and resolve them before they become critical problems.</t>
+  </si>
+  <si>
+    <t>Sending an agenda ahead of time will allow your committee members to better prepare to present on any items they need to discuss, as well as allowing for your meetings to run more efficiently.</t>
+  </si>
+  <si>
+    <t>Roundtable is your unit's link back to the district for updates, information, and idea sharing. You should have at least one representative attend each roundtable to report back to the unit.</t>
+  </si>
+  <si>
+    <t>Specific training for the outdoor activities in your program area are critical for providing a safe program. Make sure your required leaders are trained and certified to protect your scouts and yourselves.</t>
+  </si>
+  <si>
+    <t>The JTE program allows you to self-evaluate year-over-year progress and judge the quality of your program against a known set of indicators. Consider participating even if you don't submit the results.</t>
+  </si>
+  <si>
+    <t>Merit Badge Colleges are a perfect opportunity to earn advancement in some of the less common merit badges. Push these events whenever possible to allow your scouts to have the best experience possible</t>
+  </si>
+  <si>
+    <t>Contacting scouts that stop attending meetings is the best way to obtain critical feedback that may indicate issues with leadership, program, or other areas that need to be addressed. A simple call or email is all it takes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consider working with your district or council to "get the word out" to your community about hwat your unit is doing. This will help with fundraising and with recruitment. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,16 +470,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -345,18 +523,197 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,68 +1028,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304E5C17-0B9C-429C-9399-47BBA4547843}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -755,6 +1146,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -763,14 +1155,47 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="72.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="22"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -793,10 +1218,322 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56480DFD-7E94-4747-B984-12F82A3A104B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="5">
+        <v>50</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D31FBBB5-6362-478A-A2DE-D9F67576EE65}">
+          <x14:formula1>
+            <xm:f>Lists!$G$2:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3884A4C6-0C22-439F-97B9-564976E21EDB}">
+          <x14:formula1>
+            <xm:f>Lists!$R$2:$R$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E8CEB5A7-E93A-42B6-B5A3-652F09A4B9C1}">
+          <x14:formula1>
+            <xm:f>Lists!$M$2:$M$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA2C7C43-158C-48B0-ADF0-DC97D9EF36F2}">
+          <x14:formula1>
+            <xm:f>Lists!$L$2:$L$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B19</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACBA8D74-11A8-4CA1-BADF-00B4539ED3DE}">
+          <x14:formula1>
+            <xm:f>Lists!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0DC08589-4A6F-42E4-9862-FA8FE1ED9761}">
+          <x14:formula1>
+            <xm:f>Lists!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16BEEA6C-7E8D-4BF0-9F43-2E9F3E8B46CB}">
+          <x14:formula1>
+            <xm:f>Lists!$O$2:$O$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC14C61E-B283-4B37-B2F7-E2284B6CD036}">
+          <x14:formula1>
+            <xm:f>Lists!A1:A4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C910F9-75D5-4278-8052-70B386A9DB23}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1051,12 +1788,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5657E4D-497E-4BE6-B1D6-8C3F18100D78}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1064,48 +1800,70 @@
     <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>19</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
@@ -1155,71 +1913,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45EA4216-6536-4916-99CB-7E50A7CD262B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1251,6 +2021,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1273,185 +2044,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D1303A-8C86-47CC-AB36-4F4CE8E6918D}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:A23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3166B7-E7C6-46E3-8B6A-C45C04E6BA1E}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1465,6 +2131,150 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D1303A-8C86-47CC-AB36-4F4CE8E6918D}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1472,70 +2282,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799E1DF0-34EF-4A6B-B5CC-FA7FF407445C}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>64</v>
+      <c r="B11" s="25" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
@@ -1603,45 +2440,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABE9E36-0B47-4379-8F26-AD7C935C1EF8}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>68</v>
+      <c r="B6" s="24" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1649,40 +2498,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAF1BBE-FF00-4E64-B621-E6411C4DF1F3}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
+      <c r="B5" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1691,38 +2557,94 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>75</v>
-      </c>
+      <c r="B5" s="22"/>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="22"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="22"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>